<commit_message>
Atualizaçãdo ta tabela de cronograma
</commit_message>
<xml_diff>
--- a/mac0499/progresso.xlsx
+++ b/mac0499/progresso.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisasilva/Documents/Sources/elurso.github.io/mac0499/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisa/Documents/Sources/elurso.github.io/mac0499/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D7D9A8-127F-CF46-84A4-0FAE4A80198C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE8C912-8B7C-4C46-BB04-5459AC3C0491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11440" yWindow="24000" windowWidth="41480" windowHeight="17360" xr2:uid="{B91B75DB-EE1E-8047-9D48-71E8249731F1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{B91B75DB-EE1E-8047-9D48-71E8249731F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="34">
   <si>
     <t>Desenvolvimento do núcleo (depende de 3 e 5)</t>
   </si>
@@ -76,12 +76,6 @@
   </si>
   <si>
     <t>Nota</t>
-  </si>
-  <si>
-    <t>Aguardando entrega</t>
-  </si>
-  <si>
-    <t>Depende de 2</t>
   </si>
   <si>
     <t>Id</t>
@@ -265,12 +259,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -280,6 +268,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,7 +622,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,88 +635,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
+      <c r="E1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="7">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="5">
         <f>DATE(2021,1,1)</f>
         <v>44197</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="5">
         <f t="shared" ref="F2:Q2" si="0">EDATE(E2,1)</f>
         <v>44228</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="5">
         <f t="shared" si="0"/>
         <v>44256</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="5">
         <f t="shared" si="0"/>
         <v>44287</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="5">
         <f t="shared" si="0"/>
         <v>44317</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="6">
         <f t="shared" si="0"/>
         <v>44348</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="6">
         <f t="shared" si="0"/>
         <v>44378</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="6">
         <f t="shared" si="0"/>
         <v>44409</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="6">
         <f t="shared" si="0"/>
         <v>44440</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="6">
         <f t="shared" si="0"/>
         <v>44470</v>
       </c>
-      <c r="O2" s="8">
+      <c r="O2" s="6">
         <f t="shared" si="0"/>
         <v>44501</v>
       </c>
-      <c r="P2" s="8">
+      <c r="P2" s="6">
         <f t="shared" si="0"/>
         <v>44531</v>
       </c>
-      <c r="Q2" s="8">
+      <c r="Q2" s="6">
         <f t="shared" si="0"/>
         <v>44562</v>
       </c>
@@ -733,31 +727,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="11"/>
+      <c r="E3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="9"/>
     </row>
     <row r="4" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
@@ -765,31 +759,29 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="11"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="9"/>
     </row>
     <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
@@ -797,33 +789,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="9"/>
     </row>
     <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
@@ -831,31 +821,31 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="11"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="9"/>
     </row>
     <row r="7" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
@@ -863,31 +853,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="11"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="9"/>
     </row>
     <row r="8" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
@@ -895,31 +885,31 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="9"/>
     </row>
     <row r="9" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
@@ -933,27 +923,27 @@
         <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="9"/>
     </row>
     <row r="10" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
@@ -967,25 +957,25 @@
         <v>12</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="N10" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="9"/>
     </row>
     <row r="11" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
@@ -999,23 +989,23 @@
         <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="9"/>
     </row>
     <row r="12" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
@@ -1029,25 +1019,25 @@
         <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="O12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="9"/>
     </row>
     <row r="13" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
@@ -1061,27 +1051,27 @@
         <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="O13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="P13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q13" s="11"/>
+        <v>25</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q13" s="9"/>
     </row>
     <row r="14" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
@@ -1095,25 +1085,25 @@
         <v>12</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="P14" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q14" s="11"/>
+        <v>25</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
@@ -1127,22 +1117,22 @@
         <v>12</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="11" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="18" x14ac:dyDescent="0.2">
@@ -1157,43 +1147,43 @@
         <v>12</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q16" s="11"/>
+        <v>25</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q16" s="9"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>11</v>
@@ -1201,10 +1191,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>